<commit_message>
Se modifico la parte de Consultas-Empleado. En para mostrar el SDI en IMSS y la fecha de baja en caso de que tenga
</commit_message>
<xml_diff>
--- a/Payroll/Content/FilesCargaMasivaIncidencias/FormatoDeIncidencias/Layout_Carga_Incidencias.xlsx
+++ b/Payroll/Content/FilesCargaMasivaIncidencias/FormatoDeIncidencias/Layout_Carga_Incidencias.xlsx
@@ -9,14 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Incidencia" sheetId="1" r:id="rId1"/>
     <sheet name="Ausentismo" sheetId="3" r:id="rId2"/>
     <sheet name="Infonavit" sheetId="4" r:id="rId3"/>
     <sheet name="PensiónAlimenticia" sheetId="5" r:id="rId4"/>
-    <sheet name="EJEMPLOS" sheetId="2" state="hidden" r:id="rId5"/>
+    <sheet name="EJEMPLOS" sheetId="2" r:id="rId5"/>
+    <sheet name="TABLAS" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Ausentismo!$A$1:$J$1</definedName>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="98">
   <si>
     <t>Empresa_id</t>
   </si>
@@ -118,6 +119,235 @@
   <si>
     <t>Aplica_En_Finiquito</t>
   </si>
+  <si>
+    <t>Bono de productividad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EJEMPLO PARA CARGA DE INCIDENCIAS </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Prueba de cargas masivas </t>
+  </si>
+  <si>
+    <t>Debe ir el numero de la empresa</t>
+  </si>
+  <si>
+    <t>Debe ir el numero del empleado</t>
+  </si>
+  <si>
+    <t>Numero de plazos que se daran al renglon, pero en caso de renglones de numero de dias debe ser = 1</t>
+  </si>
+  <si>
+    <t>Será el monto a aplicar en el renglon exeptuando los renglones de dias donde en ese caso sera monto = 0</t>
+  </si>
+  <si>
+    <t>Este contiene el numero de dias que aplica del renglon en caso contrario es = 0</t>
+  </si>
+  <si>
+    <t>Debe ir el numero de renglón a cargar</t>
+  </si>
+  <si>
+    <t>Aquí ira en preferentemente el nombre del renglon para tenerlo como referencia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0 = No aplica en finiquito
+1 = Si aplica a finiquito
+</t>
+  </si>
+  <si>
+    <t>EJEMPLO PARA CARGA DE AUSENTISMOS</t>
+  </si>
+  <si>
+    <t>1 Accidente de Trabajo</t>
+  </si>
+  <si>
+    <t>2 Adopción Infante</t>
+  </si>
+  <si>
+    <t>3 Ausentismo fraccionado</t>
+  </si>
+  <si>
+    <t>4 Castigo y Suspension</t>
+  </si>
+  <si>
+    <t>5 Devolucion ausencia justificada</t>
+  </si>
+  <si>
+    <t>6 Enfermedad General</t>
+  </si>
+  <si>
+    <t>7 Enfermedad General Continuidad</t>
+  </si>
+  <si>
+    <t>8 Fallecimiento Padres, Hermanos, Conyugues, Concubina e Hijos</t>
+  </si>
+  <si>
+    <t>9 Faltas Injustificada</t>
+  </si>
+  <si>
+    <t>10 Lactancia</t>
+  </si>
+  <si>
+    <t>11 Matrimonio</t>
+  </si>
+  <si>
+    <t>12 Nacimiento Hijos o Adopción</t>
+  </si>
+  <si>
+    <t>13 Onomastico</t>
+  </si>
+  <si>
+    <t>14 Permiso con Sueldo</t>
+  </si>
+  <si>
+    <t>15 Permiso sin Sueldo</t>
+  </si>
+  <si>
+    <t>16 Post Quirurjico</t>
+  </si>
+  <si>
+    <t>17 Postnatal</t>
+  </si>
+  <si>
+    <t>18 Prenatal</t>
+  </si>
+  <si>
+    <t>19 Retardos</t>
+  </si>
+  <si>
+    <t>20 Riesgo de Trabajo</t>
+  </si>
+  <si>
+    <t>21 Salidas por Negocio</t>
+  </si>
+  <si>
+    <t>TIPOS DE AUSENTISMO</t>
+  </si>
+  <si>
+    <t>Falta injustificada</t>
+  </si>
+  <si>
+    <t>Solo aplica en caso de que sea una incapacidad en caso contrario dejar en blanco</t>
+  </si>
+  <si>
+    <t>Este contiene el numero de dias que aplica el ausentismo</t>
+  </si>
+  <si>
+    <t>DEJAR EN BLANCO</t>
+  </si>
+  <si>
+    <r>
+      <t>Esta referencia sera para diferenciar la carga e identificar cada carga (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>DE PREFERENCIA SEA DIFERENTE EN CADA LAYOUT CARGADO</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>Se debera poner en formato dd/mm/aaaa</t>
+  </si>
+  <si>
+    <t>Se tiene una pestaña llamada tablas al lado derecho para revizar que tipo de ausentismo aplicaria</t>
+  </si>
+  <si>
+    <t>1 En cada periodo</t>
+  </si>
+  <si>
+    <t>CR123414</t>
+  </si>
+  <si>
+    <t>Se tiene una pestaña llamada tablas al lado derecho para revizar que tipo de descuento aplicaria</t>
+  </si>
+  <si>
+    <t>1 Cuota fija</t>
+  </si>
+  <si>
+    <t>Se tiene una pestaña llamada tablas al lado derecho para revizar que opcion aplicaria</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sera el monto mensual a aplicar en caso de cuota fija, en caso de porcentaje sera un numero desde 1.00 a 99.00, en caso de Cuota fija sobre UMA la cantidad de este campo será el factor  </t>
+  </si>
+  <si>
+    <t>EJEMPLO PARA CARGA DE CREDITOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Debe ir el folio del documento proporcionado </t>
+  </si>
+  <si>
+    <t>2 Porcentaje</t>
+  </si>
+  <si>
+    <t>3 N veces en salario minimo</t>
+  </si>
+  <si>
+    <t>4 Cuota fija sobre UMA</t>
+  </si>
+  <si>
+    <t>TIPO DESCUENTO</t>
+  </si>
+  <si>
+    <t>2 En primer periodo del mes</t>
+  </si>
+  <si>
+    <t>3 En el ultimo periodo del mes</t>
+  </si>
+  <si>
+    <t>DESCONTAR EN</t>
+  </si>
+  <si>
+    <t>APLICA EN</t>
+  </si>
+  <si>
+    <t>340 Nomina</t>
+  </si>
+  <si>
+    <t>341 Finiquito</t>
+  </si>
+  <si>
+    <t>342 Aguinaldo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Monto mensual que se pedira para el credito, en caso de que sea un porcentaje el campo debe quedar  = 0 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sera el porcentaje a descontar del salario mensual, en caso de que credito sea de cuota fija el campo debe ser = 0 </t>
+  </si>
+  <si>
+    <t>Se esta trabajando para que este campo sea por default para las empresas</t>
+  </si>
+  <si>
+    <t>En caso de que tenga ira el nombre completo de la beneficiaria</t>
+  </si>
+  <si>
+    <t>(Opcional)El numero del banco que se utilizara para el pago</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Opcional) Sera la sucursal que marque el banco en caso que tenga </t>
+  </si>
+  <si>
+    <t>(Opcional) Numero de tarjeta de vales en caso de aplicar</t>
+  </si>
+  <si>
+    <t>(Opcional) Numero de cuenta de cheques en caso de aplicar</t>
+  </si>
 </sst>
 </file>
 
@@ -126,7 +356,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -163,8 +393,39 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FFFFFF00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -177,8 +438,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -230,12 +509,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -262,6 +556,41 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Millares" xfId="1" builtinId="3"/>
@@ -579,8 +908,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I122"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -997,7 +1326,7 @@
   <dimension ref="A1:J217"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1706,7 +2035,7 @@
   <dimension ref="A1:J1365"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8584,8 +8913,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N95"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection sqref="A1:N1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9035,32 +9364,628 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:N18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.42578125" customWidth="1"/>
-    <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.140625" customWidth="1"/>
+    <col min="6" max="6" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.140625" customWidth="1"/>
+    <col min="13" max="13" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="31" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="21.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="6" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="7" ht="29.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="1" spans="1:14" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="F1" s="24"/>
+      <c r="G1" s="24"/>
+      <c r="H1" s="24"/>
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+    </row>
+    <row r="2" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="15">
+        <v>4</v>
+      </c>
+      <c r="B3" s="15">
+        <v>10000</v>
+      </c>
+      <c r="C3" s="15">
+        <v>1</v>
+      </c>
+      <c r="D3" s="15">
+        <v>355.94</v>
+      </c>
+      <c r="E3" s="15">
+        <v>0</v>
+      </c>
+      <c r="F3" s="15">
+        <v>607</v>
+      </c>
+      <c r="G3" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="H3" s="15">
+        <v>0</v>
+      </c>
+      <c r="I3" s="15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" s="14" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A4" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>37</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>38</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="H4" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="I4" s="14" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="B6" s="24"/>
+      <c r="C6" s="24"/>
+      <c r="D6" s="24"/>
+      <c r="E6" s="24"/>
+      <c r="F6" s="24"/>
+      <c r="G6" s="24"/>
+      <c r="H6" s="24"/>
+      <c r="I6" s="24"/>
+      <c r="J6" s="24"/>
+    </row>
+    <row r="7" spans="1:14" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="16">
+        <v>4</v>
+      </c>
+      <c r="B8" s="16">
+        <v>10000</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>50</v>
+      </c>
+      <c r="D8" s="17">
+        <v>44180</v>
+      </c>
+      <c r="E8" s="16">
+        <v>3</v>
+      </c>
+      <c r="F8" s="16"/>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="I8" s="16">
+        <v>0</v>
+      </c>
+      <c r="J8" s="15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="90" x14ac:dyDescent="0.25">
+      <c r="A9" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="G9" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="H9" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="I9" s="14" t="s">
+        <v>40</v>
+      </c>
+      <c r="J9" s="14" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="A11" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="B11" s="24"/>
+      <c r="C11" s="24"/>
+      <c r="D11" s="24"/>
+      <c r="E11" s="24"/>
+      <c r="F11" s="24"/>
+      <c r="G11" s="24"/>
+      <c r="H11" s="24"/>
+      <c r="I11" s="24"/>
+      <c r="J11" s="24"/>
+    </row>
+    <row r="12" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" s="15" customFormat="1" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="15">
+        <v>4</v>
+      </c>
+      <c r="B13" s="15">
+        <v>10000</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="E13" s="15">
+        <v>5000</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="G13" s="20">
+        <v>44180</v>
+      </c>
+      <c r="I13" s="15">
+        <v>0</v>
+      </c>
+      <c r="J13" s="15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" s="25" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B14" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="D14" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="E14" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="F14" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="G14" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="H14" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="I14" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="J14" s="14" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="A16" s="24" t="s">
+        <v>77</v>
+      </c>
+      <c r="B16" s="24"/>
+      <c r="C16" s="24"/>
+      <c r="D16" s="24"/>
+      <c r="E16" s="24"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="24"/>
+      <c r="H16" s="24"/>
+      <c r="I16" s="24"/>
+      <c r="J16" s="24"/>
+      <c r="K16" s="24"/>
+      <c r="L16" s="24"/>
+      <c r="M16" s="24"/>
+      <c r="N16" s="24"/>
+    </row>
+    <row r="17" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K17" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="L17" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M17" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="N17" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" s="25" customFormat="1" ht="90.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="25">
+        <v>4</v>
+      </c>
+      <c r="B18" s="25">
+        <v>10000</v>
+      </c>
+      <c r="C18" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="D18" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="E18" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="F18" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="G18" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="H18" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="I18" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="J18" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="K18" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="L18" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="M18" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="N18" s="14" t="s">
+        <v>68</v>
+      </c>
+    </row>
   </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A6:J6"/>
+    <mergeCell ref="A11:J11"/>
+    <mergeCell ref="A16:N16"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="59.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>85</v>
+      </c>
+      <c r="G1" s="19" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>74</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>71</v>
+      </c>
+      <c r="G2" s="18" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="G3" s="18" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="G4" s="18" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="18" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="18" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="D8" s="23"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="18" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="18" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="18" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="18" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="18" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="18" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="18" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="18" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="18" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="18" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="18" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="18" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="18" t="s">
+        <v>62</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Actualizacion de la carga masiva 2.0
</commit_message>
<xml_diff>
--- a/Payroll/Content/FilesCargaMasivaIncidencias/FormatoDeIncidencias/Layout_Carga_Incidencias.xlsx
+++ b/Payroll/Content/FilesCargaMasivaIncidencias/FormatoDeIncidencias/Layout_Carga_Incidencias.xlsx
@@ -9,15 +9,15 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="4"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Incidencia" sheetId="1" r:id="rId1"/>
     <sheet name="Ausentismo" sheetId="3" r:id="rId2"/>
     <sheet name="Infonavit" sheetId="4" r:id="rId3"/>
     <sheet name="PensiónAlimenticia" sheetId="5" r:id="rId4"/>
-    <sheet name="EJEMPLOS" sheetId="2" r:id="rId5"/>
-    <sheet name="TABLAS" sheetId="6" r:id="rId6"/>
+    <sheet name="TABLAS" sheetId="6" r:id="rId5"/>
+    <sheet name="EJEMPLOS" sheetId="2" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Ausentismo!$A$1:$J$1</definedName>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="101">
   <si>
     <t>Empresa_id</t>
   </si>
@@ -268,16 +268,10 @@
     <t>Se tiene una pestaña llamada tablas al lado derecho para revizar que tipo de ausentismo aplicaria</t>
   </si>
   <si>
-    <t>1 En cada periodo</t>
-  </si>
-  <si>
     <t>CR123414</t>
   </si>
   <si>
     <t>Se tiene una pestaña llamada tablas al lado derecho para revizar que tipo de descuento aplicaria</t>
-  </si>
-  <si>
-    <t>1 Cuota fija</t>
   </si>
   <si>
     <t>Se tiene una pestaña llamada tablas al lado derecho para revizar que opcion aplicaria</t>
@@ -292,22 +286,7 @@
     <t xml:space="preserve">Debe ir el folio del documento proporcionado </t>
   </si>
   <si>
-    <t>2 Porcentaje</t>
-  </si>
-  <si>
-    <t>3 N veces en salario minimo</t>
-  </si>
-  <si>
-    <t>4 Cuota fija sobre UMA</t>
-  </si>
-  <si>
     <t>TIPO DESCUENTO</t>
-  </si>
-  <si>
-    <t>2 En primer periodo del mes</t>
-  </si>
-  <si>
-    <t>3 En el ultimo periodo del mes</t>
   </si>
   <si>
     <t>DESCONTAR EN</t>
@@ -348,6 +327,36 @@
   <si>
     <t>(Opcional) Numero de cuenta de cheques en caso de aplicar</t>
   </si>
+  <si>
+    <t xml:space="preserve">Para dudas o aclaraciones con Oscar Mejia - Sistemas </t>
+  </si>
+  <si>
+    <t>289 Cuota fija</t>
+  </si>
+  <si>
+    <t>290 Porcentaje</t>
+  </si>
+  <si>
+    <t>291 N veces en salario minimo</t>
+  </si>
+  <si>
+    <t>292 Cuota fija sobre UMA</t>
+  </si>
+  <si>
+    <t>314 En cada periodo</t>
+  </si>
+  <si>
+    <t>315 En primer periodo del mes</t>
+  </si>
+  <si>
+    <t>316 En el ultimo periodo del mes</t>
+  </si>
+  <si>
+    <t>EJEMPLO PARA CARGA DE PENSIONES ALIMENTICIAS</t>
+  </si>
+  <si>
+    <t>298 Cuota fija</t>
+  </si>
 </sst>
 </file>
 
@@ -356,7 +365,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -424,8 +433,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -453,6 +470,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -529,7 +552,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -582,14 +605,18 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -9364,10 +9391,183 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N18"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="59.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="E1" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="G1" s="19" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="E2" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="G2" s="18" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="C3" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="E3" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="G3" s="18" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="E4" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="G4" s="18" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="18" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="18" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="18" t="s">
+        <v>47</v>
+      </c>
+      <c r="E7" s="13"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="18" t="s">
+        <v>48</v>
+      </c>
+      <c r="D8" s="23"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="18" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="18" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="18" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="18" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="18" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="18" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="18" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="18" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="18" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18" s="18" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19" s="18" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A20" s="18" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A21" s="18" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A22" s="18" t="s">
+        <v>62</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9387,605 +9587,451 @@
     <col min="14" max="14" width="31" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="24" t="s">
+    <row r="1" spans="1:12" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="28" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="28"/>
+      <c r="I1" s="28"/>
+      <c r="J1" s="28"/>
+      <c r="K1" s="28"/>
+      <c r="L1" s="26"/>
+    </row>
+    <row r="2" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="27" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="24"/>
-      <c r="C1" s="24"/>
-      <c r="D1" s="24"/>
-      <c r="E1" s="24"/>
-      <c r="F1" s="24"/>
-      <c r="G1" s="24"/>
-      <c r="H1" s="24"/>
-      <c r="I1" s="24"/>
-      <c r="J1" s="24"/>
-    </row>
-    <row r="2" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="27"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="27"/>
+      <c r="H2" s="27"/>
+      <c r="I2" s="27"/>
+      <c r="J2" s="27"/>
+    </row>
+    <row r="3" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="F3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H2" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I3" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:14" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="15">
+    <row r="4" spans="1:12" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="15">
         <v>4</v>
       </c>
-      <c r="B3" s="15">
+      <c r="B4" s="15">
         <v>10000</v>
       </c>
-      <c r="C3" s="15">
+      <c r="C4" s="15">
         <v>1</v>
       </c>
-      <c r="D3" s="15">
+      <c r="D4" s="15">
         <v>355.94</v>
       </c>
-      <c r="E3" s="15">
+      <c r="E4" s="15">
         <v>0</v>
       </c>
-      <c r="F3" s="15">
+      <c r="F4" s="15">
         <v>607</v>
       </c>
-      <c r="G3" s="15" t="s">
+      <c r="G4" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="H3" s="15">
+      <c r="H4" s="15">
         <v>0</v>
       </c>
-      <c r="I3" s="15" t="s">
+      <c r="I4" s="15" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:14" s="14" customFormat="1" ht="90" x14ac:dyDescent="0.25">
-      <c r="A4" s="14" t="s">
+    <row r="5" spans="1:12" s="14" customFormat="1" ht="90" x14ac:dyDescent="0.25">
+      <c r="A5" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B5" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C5" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="D4" s="14" t="s">
+      <c r="D5" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="E4" s="14" t="s">
+      <c r="E5" s="14" t="s">
         <v>37</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="F5" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="G4" s="14" t="s">
+      <c r="G5" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="H4" s="14" t="s">
+      <c r="H5" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="I4" s="14" t="s">
+      <c r="I5" s="14" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="24" t="s">
+    <row r="7" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="B6" s="24"/>
-      <c r="C6" s="24"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
-      <c r="F6" s="24"/>
-      <c r="G6" s="24"/>
-      <c r="H6" s="24"/>
-      <c r="I6" s="24"/>
-      <c r="J6" s="24"/>
-    </row>
-    <row r="7" spans="1:14" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
+      <c r="B7" s="27"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="27"/>
+      <c r="E7" s="27"/>
+      <c r="F7" s="27"/>
+      <c r="G7" s="27"/>
+      <c r="H7" s="27"/>
+      <c r="I7" s="27"/>
+      <c r="J7" s="27"/>
+    </row>
+    <row r="8" spans="1:12" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B8" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F8" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="G8" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="H8" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="I7" s="2" t="s">
+      <c r="I8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="J7" s="3" t="s">
+      <c r="J8" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:14" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="16">
+    <row r="9" spans="1:12" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="16">
         <v>4</v>
       </c>
-      <c r="B8" s="16">
+      <c r="B9" s="16">
         <v>10000</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C9" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="D8" s="17">
+      <c r="D9" s="17">
         <v>44180</v>
       </c>
-      <c r="E8" s="16">
+      <c r="E9" s="16">
         <v>3</v>
       </c>
-      <c r="F8" s="16"/>
-      <c r="G8" s="16"/>
-      <c r="H8" s="16" t="s">
+      <c r="F9" s="16"/>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="I8" s="16">
+      <c r="I9" s="16">
         <v>0</v>
       </c>
-      <c r="J8" s="15" t="s">
+      <c r="J9" s="15" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:14" ht="90" x14ac:dyDescent="0.25">
-      <c r="A9" s="14" t="s">
+    <row r="10" spans="1:12" ht="90" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B10" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C10" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="D10" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="E10" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="F9" s="14" t="s">
+      <c r="F10" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="G9" s="14" t="s">
+      <c r="G10" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="H9" s="14" t="s">
+      <c r="H10" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="I9" s="14" t="s">
+      <c r="I10" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="J9" s="14" t="s">
+      <c r="J10" s="14" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="21" x14ac:dyDescent="0.25">
-      <c r="A11" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="B11" s="24"/>
-      <c r="C11" s="24"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
-      <c r="F11" s="24"/>
-      <c r="G11" s="24"/>
-      <c r="H11" s="24"/>
-      <c r="I11" s="24"/>
-      <c r="J11" s="24"/>
-    </row>
-    <row r="12" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="1" t="s">
+    <row r="12" spans="1:12" ht="21" x14ac:dyDescent="0.25">
+      <c r="A12" s="27" t="s">
+        <v>75</v>
+      </c>
+      <c r="B12" s="27"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="27"/>
+      <c r="E12" s="27"/>
+      <c r="F12" s="27"/>
+      <c r="G12" s="27"/>
+      <c r="H12" s="27"/>
+      <c r="I12" s="27"/>
+      <c r="J12" s="27"/>
+    </row>
+    <row r="13" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B13" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C13" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D13" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="E12" s="5" t="s">
+      <c r="E13" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="F12" s="8" t="s">
+      <c r="F13" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="G12" s="5" t="s">
+      <c r="G13" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="H12" s="5" t="s">
+      <c r="H13" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="I12" s="2" t="s">
+      <c r="I13" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="J12" s="3" t="s">
+      <c r="J13" s="3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="1:14" s="15" customFormat="1" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="15">
+    <row r="14" spans="1:12" s="15" customFormat="1" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="15">
         <v>4</v>
       </c>
-      <c r="B13" s="15">
+      <c r="B14" s="15">
         <v>10000</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C14" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="E14" s="15">
+        <v>5000</v>
+      </c>
+      <c r="F14" s="15" t="s">
+        <v>71</v>
+      </c>
+      <c r="G14" s="20">
+        <v>44180</v>
+      </c>
+      <c r="I14" s="15">
+        <v>0</v>
+      </c>
+      <c r="J14" s="15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" s="24" customFormat="1" ht="105" x14ac:dyDescent="0.25">
+      <c r="A15" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="B15" s="14" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="D15" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="E15" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="D13" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="E13" s="15">
-        <v>5000</v>
-      </c>
-      <c r="F13" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="G13" s="20">
-        <v>44180</v>
-      </c>
-      <c r="I13" s="15">
+      <c r="F15" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="G15" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="H15" s="21" t="s">
+        <v>67</v>
+      </c>
+      <c r="I15" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="J15" s="14" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="A17" s="27" t="s">
+        <v>99</v>
+      </c>
+      <c r="B17" s="27"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="27"/>
+      <c r="E17" s="27"/>
+      <c r="F17" s="27"/>
+      <c r="G17" s="27"/>
+      <c r="H17" s="27"/>
+      <c r="I17" s="27"/>
+      <c r="J17" s="27"/>
+      <c r="K17" s="27"/>
+      <c r="L17" s="27"/>
+      <c r="M17" s="27"/>
+      <c r="N17" s="27"/>
+    </row>
+    <row r="18" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="J13" s="15" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" s="25" customFormat="1" ht="105" x14ac:dyDescent="0.25">
-      <c r="A14" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="B14" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="C14" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="D14" s="14" t="s">
-        <v>75</v>
-      </c>
-      <c r="E14" s="14" t="s">
+      <c r="B18" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="K18" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="L18" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M18" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="N18" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" s="24" customFormat="1" ht="90.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="24">
+        <v>4</v>
+      </c>
+      <c r="B19" s="24">
+        <v>10000</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="D19" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="E19" s="25" t="s">
+        <v>85</v>
+      </c>
+      <c r="F19" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="F14" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="G14" s="14" t="s">
+      <c r="G19" s="14" t="s">
         <v>69</v>
       </c>
-      <c r="H14" s="21" t="s">
-        <v>67</v>
-      </c>
-      <c r="I14" s="22" t="s">
+      <c r="H19" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="I19" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="J19" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="K19" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="L19" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="M19" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="J14" s="14" t="s">
+      <c r="N19" s="14" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="16" spans="1:14" ht="21" x14ac:dyDescent="0.25">
-      <c r="A16" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="B16" s="24"/>
-      <c r="C16" s="24"/>
-      <c r="D16" s="24"/>
-      <c r="E16" s="24"/>
-      <c r="F16" s="24"/>
-      <c r="G16" s="24"/>
-      <c r="H16" s="24"/>
-      <c r="I16" s="24"/>
-      <c r="J16" s="24"/>
-      <c r="K16" s="24"/>
-      <c r="L16" s="24"/>
-      <c r="M16" s="24"/>
-      <c r="N16" s="24"/>
-    </row>
-    <row r="17" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E17" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F17" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="I17" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="J17" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="K17" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="L17" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="M17" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="N17" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" s="25" customFormat="1" ht="90.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="25">
-        <v>4</v>
-      </c>
-      <c r="B18" s="25">
-        <v>10000</v>
-      </c>
-      <c r="C18" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="D18" s="14" t="s">
-        <v>91</v>
-      </c>
-      <c r="E18" s="26" t="s">
-        <v>92</v>
-      </c>
-      <c r="F18" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="G18" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="H18" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="I18" s="14" t="s">
-        <v>94</v>
-      </c>
-      <c r="J18" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="K18" s="14" t="s">
-        <v>97</v>
-      </c>
-      <c r="L18" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="M18" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="N18" s="14" t="s">
-        <v>68</v>
-      </c>
-    </row>
   </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A6:J6"/>
-    <mergeCell ref="A11:J11"/>
-    <mergeCell ref="A16:N16"/>
+  <mergeCells count="5">
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A7:J7"/>
+    <mergeCell ref="A12:J12"/>
+    <mergeCell ref="A17:N17"/>
+    <mergeCell ref="A1:K1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G22"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="59.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.28515625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="19" t="s">
-        <v>63</v>
-      </c>
-      <c r="C1" s="19" t="s">
-        <v>82</v>
-      </c>
-      <c r="E1" s="19" t="s">
-        <v>85</v>
-      </c>
-      <c r="G1" s="19" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="C2" s="18" t="s">
-        <v>74</v>
-      </c>
-      <c r="E2" s="18" t="s">
-        <v>71</v>
-      </c>
-      <c r="G2" s="18" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="18" t="s">
-        <v>43</v>
-      </c>
-      <c r="C3" s="18" t="s">
-        <v>79</v>
-      </c>
-      <c r="E3" s="18" t="s">
-        <v>83</v>
-      </c>
-      <c r="G3" s="18" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="18" t="s">
-        <v>44</v>
-      </c>
-      <c r="C4" s="18" t="s">
-        <v>80</v>
-      </c>
-      <c r="E4" s="18" t="s">
-        <v>84</v>
-      </c>
-      <c r="G4" s="18" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A5" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="C5" s="18" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="18" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="18" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="18" t="s">
-        <v>48</v>
-      </c>
-      <c r="D8" s="23"/>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="18" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" s="18" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" s="18" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="18" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" s="18" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="18" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="18" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="18" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="18" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A18" s="18" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A19" s="18" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A20" s="18" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A21" s="18" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A22" s="18" t="s">
-        <v>62</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
CARGA DE VACACIONES MASIVA CON NUEVO LAYOUT
</commit_message>
<xml_diff>
--- a/Payroll/Content/FilesCargaMasivaIncidencias/FormatoDeIncidencias/Layout_Carga_Incidencias.xlsx
+++ b/Payroll/Content/FilesCargaMasivaIncidencias/FormatoDeIncidencias/Layout_Carga_Incidencias.xlsx
@@ -1,23 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23628"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Oscar Mejía Doroteo\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Oscar Mejia\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B968A41-FF9B-4157-9D9C-F319795EC172}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" tabRatio="676" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Incidencia" sheetId="1" r:id="rId1"/>
     <sheet name="Ausentismo" sheetId="3" r:id="rId2"/>
     <sheet name="Infonavit" sheetId="4" r:id="rId3"/>
     <sheet name="PensiónAlimenticia" sheetId="5" r:id="rId4"/>
-    <sheet name="TABLAS" sheetId="6" r:id="rId5"/>
-    <sheet name="EJEMPLOS" sheetId="2" r:id="rId6"/>
+    <sheet name="Vacaciones" sheetId="7" r:id="rId5"/>
+    <sheet name="TABLAS" sheetId="6" r:id="rId6"/>
+    <sheet name="EJEMPLOS" sheetId="2" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Ausentismo!$A$1:$J$1</definedName>
@@ -28,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="108">
   <si>
     <t>Empresa_id</t>
   </si>
@@ -357,11 +359,32 @@
   <si>
     <t>298 Cuota fija</t>
   </si>
+  <si>
+    <t>Año</t>
+  </si>
+  <si>
+    <t>Fecha_inicio</t>
+  </si>
+  <si>
+    <t>Fecha_fin</t>
+  </si>
+  <si>
+    <t>Dias</t>
+  </si>
+  <si>
+    <t>EJEMPLO PARA CARGA DE VACACIONES</t>
+  </si>
+  <si>
+    <t>Este es un campo opcional y se puede utilizar en caso de tenerla</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ggatada de vatos </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
@@ -435,7 +458,7 @@
     </font>
     <font>
       <b/>
-      <sz val="20"/>
+      <sz val="28"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -552,7 +575,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -612,11 +635,14 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -932,11 +958,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:I122"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="G51" sqref="G51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1343,17 +1370,18 @@
       <c r="D122" s="4"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I1"/>
+  <autoFilter ref="A1:I1" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr codeName="Hoja2"/>
   <dimension ref="A1:J217"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="G51" sqref="G51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2050,7 +2078,7 @@
       <c r="D217" s="6"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J1"/>
+  <autoFilter ref="A1:J1" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2058,11 +2086,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <sheetPr codeName="Hoja3"/>
   <dimension ref="A1:J1365"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="G51" sqref="G51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8937,11 +8966,12 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+  <sheetPr codeName="Hoja4"/>
   <dimension ref="A1:N95"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection sqref="A1:N1"/>
+    <sheetView topLeftCell="D1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G51" sqref="G51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9390,11 +9420,85 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <sheetPr codeName="Hoja5"/>
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" customWidth="1"/>
+    <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" customWidth="1"/>
+    <col min="6" max="6" width="8.5703125" customWidth="1"/>
+    <col min="7" max="7" width="67.28515625" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>4</v>
+      </c>
+      <c r="B2">
+        <v>10000</v>
+      </c>
+      <c r="C2">
+        <v>2021</v>
+      </c>
+      <c r="D2" s="6">
+        <v>44237</v>
+      </c>
+      <c r="F2">
+        <v>4</v>
+      </c>
+      <c r="G2" t="s">
+        <v>107</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+  <sheetPr codeName="Hoja6"/>
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="G51" sqref="G51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9562,12 +9666,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N19"/>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+  <sheetPr codeName="Hoja7"/>
+  <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="G51" sqref="G51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9604,18 +9709,18 @@
       <c r="L1" s="26"/>
     </row>
     <row r="2" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="27"/>
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
     </row>
     <row r="3" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
@@ -9705,18 +9810,18 @@
       </c>
     </row>
     <row r="7" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="27" t="s">
+      <c r="A7" s="29" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="27"/>
-      <c r="C7" s="27"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="27"/>
-      <c r="I7" s="27"/>
-      <c r="J7" s="27"/>
+      <c r="B7" s="29"/>
+      <c r="C7" s="29"/>
+      <c r="D7" s="29"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="29"/>
+      <c r="G7" s="29"/>
+      <c r="H7" s="29"/>
+      <c r="I7" s="29"/>
+      <c r="J7" s="29"/>
     </row>
     <row r="8" spans="1:12" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
@@ -9811,18 +9916,18 @@
       </c>
     </row>
     <row r="12" spans="1:12" ht="21" x14ac:dyDescent="0.25">
-      <c r="A12" s="27" t="s">
+      <c r="A12" s="29" t="s">
         <v>75</v>
       </c>
-      <c r="B12" s="27"/>
-      <c r="C12" s="27"/>
-      <c r="D12" s="27"/>
-      <c r="E12" s="27"/>
-      <c r="F12" s="27"/>
-      <c r="G12" s="27"/>
-      <c r="H12" s="27"/>
-      <c r="I12" s="27"/>
-      <c r="J12" s="27"/>
+      <c r="B12" s="29"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="29"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="29"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="29"/>
+      <c r="I12" s="29"/>
+      <c r="J12" s="29"/>
     </row>
     <row r="13" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
@@ -9918,22 +10023,22 @@
       </c>
     </row>
     <row r="17" spans="1:14" ht="21" x14ac:dyDescent="0.25">
-      <c r="A17" s="27" t="s">
+      <c r="A17" s="29" t="s">
         <v>99</v>
       </c>
-      <c r="B17" s="27"/>
-      <c r="C17" s="27"/>
-      <c r="D17" s="27"/>
-      <c r="E17" s="27"/>
-      <c r="F17" s="27"/>
-      <c r="G17" s="27"/>
-      <c r="H17" s="27"/>
-      <c r="I17" s="27"/>
-      <c r="J17" s="27"/>
-      <c r="K17" s="27"/>
-      <c r="L17" s="27"/>
-      <c r="M17" s="27"/>
-      <c r="N17" s="27"/>
+      <c r="B17" s="29"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="29"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="29"/>
+      <c r="G17" s="29"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="29"/>
+      <c r="J17" s="29"/>
+      <c r="K17" s="29"/>
+      <c r="L17" s="29"/>
+      <c r="M17" s="29"/>
+      <c r="N17" s="29"/>
     </row>
     <row r="18" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
@@ -10023,13 +10128,74 @@
         <v>68</v>
       </c>
     </row>
+    <row r="21" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="A21" s="29" t="s">
+        <v>105</v>
+      </c>
+      <c r="B21" s="29"/>
+      <c r="C21" s="29"/>
+      <c r="D21" s="29"/>
+      <c r="E21" s="29"/>
+      <c r="F21" s="29"/>
+      <c r="G21" s="29"/>
+      <c r="H21" s="29"/>
+      <c r="I21" s="29"/>
+      <c r="J21" s="29"/>
+    </row>
+    <row r="22" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="G22" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" s="24" customFormat="1" ht="102.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="24">
+        <v>4</v>
+      </c>
+      <c r="B23" s="24">
+        <v>10000</v>
+      </c>
+      <c r="C23" s="24">
+        <v>2021</v>
+      </c>
+      <c r="D23" s="27">
+        <v>44235</v>
+      </c>
+      <c r="E23" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F23" s="24">
+        <v>3</v>
+      </c>
+      <c r="G23" s="14" t="s">
+        <v>68</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A21:J21"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A7:J7"/>
     <mergeCell ref="A12:J12"/>
     <mergeCell ref="A17:N17"/>
-    <mergeCell ref="A1:K1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
actualizacion de modulo de catalogos - perfiles y usuarios
</commit_message>
<xml_diff>
--- a/Payroll/Content/FilesCargaMasivaIncidencias/FormatoDeIncidencias/Layout_Carga_Incidencias.xlsx
+++ b/Payroll/Content/FilesCargaMasivaIncidencias/FormatoDeIncidencias/Layout_Carga_Incidencias.xlsx
@@ -9,15 +9,16 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Incidencia" sheetId="1" r:id="rId1"/>
     <sheet name="Ausentismo" sheetId="3" r:id="rId2"/>
     <sheet name="Infonavit" sheetId="4" r:id="rId3"/>
     <sheet name="PensiónAlimenticia" sheetId="5" r:id="rId4"/>
-    <sheet name="TABLAS" sheetId="6" r:id="rId5"/>
-    <sheet name="EJEMPLOS" sheetId="2" r:id="rId6"/>
+    <sheet name="Vacaciones" sheetId="7" r:id="rId5"/>
+    <sheet name="TABLAS" sheetId="6" r:id="rId6"/>
+    <sheet name="EJEMPLOS" sheetId="2" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Ausentismo!$A$1:$J$1</definedName>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="107">
   <si>
     <t>Empresa_id</t>
   </si>
@@ -356,6 +357,24 @@
   </si>
   <si>
     <t>298 Cuota fija</t>
+  </si>
+  <si>
+    <t>Año</t>
+  </si>
+  <si>
+    <t>Fecha_inicio</t>
+  </si>
+  <si>
+    <t>Fecha_fin</t>
+  </si>
+  <si>
+    <t>Dias</t>
+  </si>
+  <si>
+    <t>EJEMPLO PARA CARGA DE VACACIONES</t>
+  </si>
+  <si>
+    <t>Este es un campo opcional y se puede utilizar en caso de tenerla</t>
   </si>
 </sst>
 </file>
@@ -435,7 +454,7 @@
     </font>
     <font>
       <b/>
-      <sz val="20"/>
+      <sz val="28"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -552,7 +571,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -612,6 +631,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -8940,7 +8962,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N95"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView topLeftCell="D1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection sqref="A1:N1"/>
     </sheetView>
   </sheetViews>
@@ -9391,10 +9413,65 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8" customWidth="1"/>
+    <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" customWidth="1"/>
+    <col min="6" max="6" width="8.5703125" customWidth="1"/>
+    <col min="7" max="7" width="67.28515625" customWidth="1"/>
+    <col min="8" max="8" width="9.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="D2" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9562,12 +9639,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N19"/>
+  <dimension ref="A1:N23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7:J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9588,34 +9665,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="29" t="s">
         <v>91</v>
       </c>
-      <c r="B1" s="28"/>
-      <c r="C1" s="28"/>
-      <c r="D1" s="28"/>
-      <c r="E1" s="28"/>
-      <c r="F1" s="28"/>
-      <c r="G1" s="28"/>
-      <c r="H1" s="28"/>
-      <c r="I1" s="28"/>
-      <c r="J1" s="28"/>
-      <c r="K1" s="28"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
       <c r="L1" s="26"/>
     </row>
     <row r="2" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="27"/>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
     </row>
     <row r="3" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
@@ -9705,18 +9782,18 @@
       </c>
     </row>
     <row r="7" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="27" t="s">
+      <c r="A7" s="28" t="s">
         <v>41</v>
       </c>
-      <c r="B7" s="27"/>
-      <c r="C7" s="27"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="27"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="27"/>
-      <c r="I7" s="27"/>
-      <c r="J7" s="27"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="28"/>
+      <c r="D7" s="28"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="28"/>
+      <c r="I7" s="28"/>
+      <c r="J7" s="28"/>
     </row>
     <row r="8" spans="1:12" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
@@ -9811,18 +9888,18 @@
       </c>
     </row>
     <row r="12" spans="1:12" ht="21" x14ac:dyDescent="0.25">
-      <c r="A12" s="27" t="s">
+      <c r="A12" s="28" t="s">
         <v>75</v>
       </c>
-      <c r="B12" s="27"/>
-      <c r="C12" s="27"/>
-      <c r="D12" s="27"/>
-      <c r="E12" s="27"/>
-      <c r="F12" s="27"/>
-      <c r="G12" s="27"/>
-      <c r="H12" s="27"/>
-      <c r="I12" s="27"/>
-      <c r="J12" s="27"/>
+      <c r="B12" s="28"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="28"/>
+      <c r="H12" s="28"/>
+      <c r="I12" s="28"/>
+      <c r="J12" s="28"/>
     </row>
     <row r="13" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
@@ -9918,22 +9995,22 @@
       </c>
     </row>
     <row r="17" spans="1:14" ht="21" x14ac:dyDescent="0.25">
-      <c r="A17" s="27" t="s">
+      <c r="A17" s="28" t="s">
         <v>99</v>
       </c>
-      <c r="B17" s="27"/>
-      <c r="C17" s="27"/>
-      <c r="D17" s="27"/>
-      <c r="E17" s="27"/>
-      <c r="F17" s="27"/>
-      <c r="G17" s="27"/>
-      <c r="H17" s="27"/>
-      <c r="I17" s="27"/>
-      <c r="J17" s="27"/>
-      <c r="K17" s="27"/>
-      <c r="L17" s="27"/>
-      <c r="M17" s="27"/>
-      <c r="N17" s="27"/>
+      <c r="B17" s="28"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="28"/>
+      <c r="G17" s="28"/>
+      <c r="H17" s="28"/>
+      <c r="I17" s="28"/>
+      <c r="J17" s="28"/>
+      <c r="K17" s="28"/>
+      <c r="L17" s="28"/>
+      <c r="M17" s="28"/>
+      <c r="N17" s="28"/>
     </row>
     <row r="18" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
@@ -10023,13 +10100,74 @@
         <v>68</v>
       </c>
     </row>
+    <row r="21" spans="1:14" ht="21" x14ac:dyDescent="0.25">
+      <c r="A21" s="28" t="s">
+        <v>105</v>
+      </c>
+      <c r="B21" s="28"/>
+      <c r="C21" s="28"/>
+      <c r="D21" s="28"/>
+      <c r="E21" s="28"/>
+      <c r="F21" s="28"/>
+      <c r="G21" s="28"/>
+      <c r="H21" s="28"/>
+      <c r="I21" s="28"/>
+      <c r="J21" s="28"/>
+    </row>
+    <row r="22" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="G22" s="9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" s="24" customFormat="1" ht="102.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="24">
+        <v>4</v>
+      </c>
+      <c r="B23" s="24">
+        <v>10000</v>
+      </c>
+      <c r="C23" s="24">
+        <v>2021</v>
+      </c>
+      <c r="D23" s="27">
+        <v>44235</v>
+      </c>
+      <c r="E23" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F23" s="24">
+        <v>3</v>
+      </c>
+      <c r="G23" s="14" t="s">
+        <v>68</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A21:J21"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A7:J7"/>
     <mergeCell ref="A12:J12"/>
     <mergeCell ref="A17:N17"/>
-    <mergeCell ref="A1:K1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
ACTUALIZACION DE LAYOUT CARGA INCIDENCIAS.
</commit_message>
<xml_diff>
--- a/Payroll/Content/FilesCargaMasivaIncidencias/FormatoDeIncidencias/Layout_Carga_Incidencias.xlsx
+++ b/Payroll/Content/FilesCargaMasivaIncidencias/FormatoDeIncidencias/Layout_Carga_Incidencias.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23628"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Oscar Mejia\Desktop\Server IPSNet\Seri\Payroll\Content\FilesCargaMasivaIncidencias\FormatoDeIncidencias\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Oscar Mejía Doroteo\Desktop\Server\Seri\Payroll\Content\FilesCargaMasivaIncidencias\FormatoDeIncidencias\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78573065-4AC8-485E-A19D-CC11BCED2264}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240"/>
   </bookViews>
   <sheets>
     <sheet name="Incidencia" sheetId="1" r:id="rId1"/>
@@ -30,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="113">
   <si>
     <t>Empresa_id</t>
   </si>
@@ -389,15 +388,22 @@
   <si>
     <t xml:space="preserve">Por default ira en cero y solo se modificara para los renglones que aplique. </t>
   </si>
+  <si>
+    <t>Periodo_especial</t>
+  </si>
+  <si>
+    <t>0 = Carga para una nomina normal
+1 = Carga para Nomina en periodo especial</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -473,8 +479,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -511,8 +524,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -594,12 +613,27 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -669,6 +703,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -989,11 +1027,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K122"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L122"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1009,11 +1047,11 @@
     <col min="9" max="9" width="23.5703125" customWidth="1"/>
     <col min="10" max="10" width="18" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="10.28515625" customWidth="1"/>
-    <col min="12" max="12" width="18" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.28515625" customWidth="1"/>
     <col min="13" max="13" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1047,50 +1085,53 @@
       <c r="K1" s="3" t="s">
         <v>109</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="L1" s="31" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="D2" s="4"/>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D3" s="4"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D4" s="4"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D5" s="4"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D6" s="4"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D7" s="4"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D8" s="4"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D9" s="4"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D10" s="4"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D11" s="4"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D12" s="4"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D13" s="4"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D14" s="4"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D15" s="4"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="D16" s="4"/>
     </row>
     <row r="17" spans="4:4" x14ac:dyDescent="0.25">
@@ -1412,17 +1453,17 @@
       <c r="D122" s="4"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I1" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:I1"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J240"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3384,7 +3425,7 @@
       <c r="J240" s="15"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:J1" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
+  <autoFilter ref="A1:J1"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -3392,7 +3433,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J1365"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -10271,7 +10312,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N95"/>
   <sheetViews>
     <sheetView topLeftCell="D1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
@@ -10724,7 +10765,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
@@ -10782,11 +10823,11 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10883,30 +10924,35 @@
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A10" s="18" t="s">
         <v>49</v>
       </c>
+      <c r="C10" s="19"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="18" t="s">
         <v>50</v>
       </c>
+      <c r="C11" s="18"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="18" t="s">
         <v>51</v>
       </c>
+      <c r="C12" s="18"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="18" t="s">
         <v>52</v>
       </c>
+      <c r="C13" s="18"/>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="18" t="s">
         <v>53</v>
       </c>
+      <c r="C14" s="18"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="18" t="s">
@@ -10955,11 +11001,11 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N23"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10974,41 +11020,42 @@
     <col min="8" max="8" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="10" width="26.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="17.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.140625" customWidth="1"/>
+    <col min="12" max="12" width="22.7109375" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="31" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="52.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="33" t="s">
         <v>90</v>
       </c>
-      <c r="B1" s="31"/>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31"/>
+      <c r="B1" s="33"/>
+      <c r="C1" s="33"/>
+      <c r="D1" s="33"/>
+      <c r="E1" s="33"/>
+      <c r="F1" s="33"/>
+      <c r="G1" s="33"/>
+      <c r="H1" s="33"/>
+      <c r="I1" s="33"/>
+      <c r="J1" s="33"/>
+      <c r="K1" s="33"/>
       <c r="L1" s="26"/>
     </row>
     <row r="2" spans="1:12" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="32" t="s">
+      <c r="A2" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="32"/>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="32"/>
-      <c r="K2" s="32"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="34"/>
+      <c r="K2" s="34"/>
+      <c r="L2" s="32"/>
     </row>
     <row r="3" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
@@ -11044,6 +11091,9 @@
       <c r="K3" s="3" t="s">
         <v>109</v>
       </c>
+      <c r="L3" s="3" t="s">
+        <v>111</v>
+      </c>
     </row>
     <row r="4" spans="1:12" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A4" s="15">
@@ -11079,6 +11129,9 @@
       <c r="K4" s="15">
         <v>0</v>
       </c>
+      <c r="L4" s="15">
+        <v>0</v>
+      </c>
     </row>
     <row r="5" spans="1:12" s="14" customFormat="1" ht="90" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
@@ -11114,20 +11167,23 @@
       <c r="K5" s="14" t="s">
         <v>110</v>
       </c>
+      <c r="L5" s="14" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="7" spans="1:12" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="32" t="s">
+      <c r="A7" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="B7" s="32"/>
-      <c r="C7" s="32"/>
-      <c r="D7" s="32"/>
-      <c r="E7" s="32"/>
-      <c r="F7" s="32"/>
-      <c r="G7" s="32"/>
-      <c r="H7" s="32"/>
-      <c r="I7" s="32"/>
-      <c r="J7" s="32"/>
+      <c r="B7" s="34"/>
+      <c r="C7" s="34"/>
+      <c r="D7" s="34"/>
+      <c r="E7" s="34"/>
+      <c r="F7" s="34"/>
+      <c r="G7" s="34"/>
+      <c r="H7" s="34"/>
+      <c r="I7" s="34"/>
+      <c r="J7" s="34"/>
     </row>
     <row r="8" spans="1:12" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
@@ -11222,18 +11278,18 @@
       </c>
     </row>
     <row r="12" spans="1:12" ht="21" x14ac:dyDescent="0.25">
-      <c r="A12" s="32" t="s">
+      <c r="A12" s="34" t="s">
         <v>74</v>
       </c>
-      <c r="B12" s="32"/>
-      <c r="C12" s="32"/>
-      <c r="D12" s="32"/>
-      <c r="E12" s="32"/>
-      <c r="F12" s="32"/>
-      <c r="G12" s="32"/>
-      <c r="H12" s="32"/>
-      <c r="I12" s="32"/>
-      <c r="J12" s="32"/>
+      <c r="B12" s="34"/>
+      <c r="C12" s="34"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="34"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="34"/>
+      <c r="I12" s="34"/>
+      <c r="J12" s="34"/>
     </row>
     <row r="13" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
@@ -11329,22 +11385,22 @@
       </c>
     </row>
     <row r="17" spans="1:14" ht="21" x14ac:dyDescent="0.25">
-      <c r="A17" s="32" t="s">
+      <c r="A17" s="34" t="s">
         <v>98</v>
       </c>
-      <c r="B17" s="32"/>
-      <c r="C17" s="32"/>
-      <c r="D17" s="32"/>
-      <c r="E17" s="32"/>
-      <c r="F17" s="32"/>
-      <c r="G17" s="32"/>
-      <c r="H17" s="32"/>
-      <c r="I17" s="32"/>
-      <c r="J17" s="32"/>
-      <c r="K17" s="32"/>
-      <c r="L17" s="32"/>
-      <c r="M17" s="32"/>
-      <c r="N17" s="32"/>
+      <c r="B17" s="34"/>
+      <c r="C17" s="34"/>
+      <c r="D17" s="34"/>
+      <c r="E17" s="34"/>
+      <c r="F17" s="34"/>
+      <c r="G17" s="34"/>
+      <c r="H17" s="34"/>
+      <c r="I17" s="34"/>
+      <c r="J17" s="34"/>
+      <c r="K17" s="34"/>
+      <c r="L17" s="34"/>
+      <c r="M17" s="34"/>
+      <c r="N17" s="34"/>
     </row>
     <row r="18" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
@@ -11435,18 +11491,18 @@
       </c>
     </row>
     <row r="21" spans="1:14" ht="21" x14ac:dyDescent="0.25">
-      <c r="A21" s="32" t="s">
+      <c r="A21" s="34" t="s">
         <v>104</v>
       </c>
-      <c r="B21" s="32"/>
-      <c r="C21" s="32"/>
-      <c r="D21" s="32"/>
-      <c r="E21" s="32"/>
-      <c r="F21" s="32"/>
-      <c r="G21" s="32"/>
-      <c r="H21" s="32"/>
-      <c r="I21" s="32"/>
-      <c r="J21" s="32"/>
+      <c r="B21" s="34"/>
+      <c r="C21" s="34"/>
+      <c r="D21" s="34"/>
+      <c r="E21" s="34"/>
+      <c r="F21" s="34"/>
+      <c r="G21" s="34"/>
+      <c r="H21" s="34"/>
+      <c r="I21" s="34"/>
+      <c r="J21" s="34"/>
     </row>
     <row r="22" spans="1:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">

</xml_diff>